<commit_message>
Updated Acceptance Test Plan with current spectator AC
</commit_message>
<xml_diff>
--- a/etc/WebCheckers Acceptance Test Plan - Grade A Slackers.xlsx
+++ b/etc/WebCheckers Acceptance Test Plan - Grade A Slackers.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2171-swen-261-04-b-Grade-A-Slackers\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Instructions" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Test Plan" sheetId="2" r:id="rId4"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="105">
   <si>
     <t>Instructions</t>
   </si>
@@ -322,70 +330,84 @@
     <t>Given that I am playing a game, when a player joins as a spectator then I expect to be able to continue playing my game as before.</t>
   </si>
   <si>
-    <t>Given that I am signed in, when I choose to spectate a game then I expect to be removed from the list of current players.</t>
-  </si>
-  <si>
     <t>Given that I am a spectator when I am viewing a game then I expect to have no permissions</t>
+  </si>
+  <si>
+    <t>Given that I have not selected a game to spectate, when I hit the spectate button then I expect to be redirected to home and given a message telling me to select a game first.</t>
+  </si>
+  <si>
+    <t>Given that I am spectating a game, when someone selects me to play a game of checkers then I expect to be given a message that I am being challenged to a game.</t>
+  </si>
+  <si>
+    <t>Given that I am spectating a game, when the game ends, then I expect to be returned to the home screen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -393,7 +415,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -414,201 +436,263 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
-    <border/>
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="58">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-      <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -620,53 +704,306 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.0"/>
-    <col customWidth="1" min="2" max="2" width="106.89"/>
-    <col customWidth="1" min="3" max="12" width="11.0"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="106.875" customWidth="1"/>
+    <col min="3" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -674,10 +1011,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -685,7 +1022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -693,88 +1030,89 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="18.75" customHeight="1">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" ht="18.75" customHeight="1">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" ht="18.75" customHeight="1">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" ht="18.75" customHeight="1">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" ht="18.75" customHeight="1">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" ht="18.75" customHeight="1">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" ht="18.75" customHeight="1">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" ht="18.75" customHeight="1">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" ht="18.75" customHeight="1">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" ht="18.75" customHeight="1">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" ht="18.75" customHeight="1">
+    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" ht="18.75" customHeight="1">
+    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" ht="18.75" customHeight="1">
+    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" ht="18.75" customHeight="1">
+    <row r="20" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" ht="18.75" customHeight="1">
+    <row r="21" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2.0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection activeCell="D2" sqref="D2" pane="topRight"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.0"/>
-    <col customWidth="1" min="2" max="2" width="60.0"/>
-    <col customWidth="1" min="3" max="3" width="9.0"/>
-    <col customWidth="1" min="4" max="4" width="60.0"/>
-    <col customWidth="1" min="5" max="5" width="9.0"/>
-    <col customWidth="1" min="6" max="6" width="60.0"/>
-    <col customWidth="1" min="7" max="7" width="9.0"/>
-    <col customWidth="1" min="8" max="8" width="60.0"/>
-    <col customWidth="1" min="9" max="9" width="10.89"/>
-    <col customWidth="1" min="10" max="10" width="46.44"/>
-    <col customWidth="1" min="11" max="11" width="10.89"/>
-    <col customWidth="1" min="12" max="12" width="36.78"/>
-    <col customWidth="1" min="13" max="18" width="10.89"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="60" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="60" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="60" customWidth="1"/>
+    <col min="9" max="9" width="10.875" customWidth="1"/>
+    <col min="10" max="10" width="46.5" customWidth="1"/>
+    <col min="11" max="11" width="10.875" customWidth="1"/>
+    <col min="12" max="12" width="36.75" customWidth="1"/>
+    <col min="13" max="18" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -818,7 +1156,7 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -853,7 +1191,7 @@
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
@@ -886,7 +1224,7 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -919,7 +1257,7 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -952,7 +1290,7 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>24</v>
@@ -985,7 +1323,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
@@ -1018,7 +1356,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>27</v>
@@ -1051,7 +1389,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>28</v>
@@ -1084,7 +1422,7 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>29</v>
@@ -1118,7 +1456,7 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
@@ -1153,7 +1491,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -1186,7 +1524,7 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>36</v>
@@ -1219,7 +1557,7 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>37</v>
@@ -1252,7 +1590,7 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>38</v>
@@ -1285,7 +1623,7 @@
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>39</v>
@@ -1318,7 +1656,7 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>40</v>
@@ -1351,7 +1689,7 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>42</v>
@@ -1385,7 +1723,7 @@
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>43</v>
       </c>
@@ -1416,7 +1754,7 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>45</v>
@@ -1445,7 +1783,7 @@
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>46</v>
@@ -1474,7 +1812,7 @@
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>47</v>
@@ -1503,7 +1841,7 @@
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30"/>
       <c r="B23" s="30" t="s">
         <v>48</v>
@@ -1533,7 +1871,7 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
@@ -1564,7 +1902,7 @@
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>51</v>
@@ -1593,7 +1931,7 @@
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
@@ -1622,7 +1960,7 @@
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>54</v>
@@ -1651,7 +1989,7 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="30" t="s">
         <v>55</v>
@@ -1681,7 +2019,7 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1708,7 +2046,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>58</v>
@@ -1737,7 +2075,7 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>59</v>
@@ -1766,7 +2104,7 @@
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>61</v>
@@ -1795,7 +2133,7 @@
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="30" t="s">
         <v>62</v>
@@ -1825,7 +2163,7 @@
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -1856,7 +2194,7 @@
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="39"/>
       <c r="B35" s="39" t="s">
         <v>66</v>
@@ -1881,7 +2219,7 @@
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42"/>
       <c r="B36" s="43" t="s">
         <v>68</v>
@@ -1911,7 +2249,7 @@
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="39" t="s">
         <v>69</v>
       </c>
@@ -1938,7 +2276,7 @@
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="46" t="s">
         <v>71</v>
       </c>
@@ -1962,7 +2300,7 @@
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="47" t="s">
         <v>72</v>
@@ -1992,7 +2330,7 @@
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
         <v>73</v>
       </c>
@@ -2012,7 +2350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" ht="28.5" customHeight="1">
+    <row r="41" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="46" t="s">
         <v>75</v>
       </c>
@@ -2029,7 +2367,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B42" s="46" t="s">
         <v>76</v>
       </c>
@@ -2046,7 +2384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B43" s="46" t="s">
         <v>77</v>
       </c>
@@ -2063,7 +2401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="24"/>
       <c r="B44" s="47" t="s">
         <v>78</v>
@@ -2087,7 +2425,7 @@
       <c r="K44" s="24"/>
       <c r="L44" s="24"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:18" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
         <v>79</v>
       </c>
@@ -2107,7 +2445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B46" s="46" t="s">
         <v>81</v>
       </c>
@@ -2124,7 +2462,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
       <c r="B47" s="47" t="s">
         <v>82</v>
@@ -2148,7 +2486,7 @@
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:18" ht="63" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
         <v>83</v>
       </c>
@@ -2156,22 +2494,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B49" s="48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B50" s="48" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B51" s="48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="49" t="s">
         <v>88</v>
@@ -2187,7 +2525,7 @@
       <c r="K52" s="24"/>
       <c r="L52" s="24"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
         <v>89</v>
       </c>
@@ -2195,40 +2533,40 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B54" s="48" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B55" s="48" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B56" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B57" s="48" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B58" s="48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="24"/>
-      <c r="B59" s="49" t="s">
+    <row r="59" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="54"/>
+      <c r="B59" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="54"/>
       <c r="G59" s="24"/>
       <c r="H59" s="24"/>
       <c r="I59" s="24"/>
@@ -2236,7 +2574,7 @@
       <c r="K59" s="24"/>
       <c r="L59" s="24"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
         <v>97</v>
       </c>
@@ -2244,83 +2582,165 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B61" s="48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B62" s="48" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B63" s="48" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="24"/>
-      <c r="B64" s="49" t="s">
+    <row r="64" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="50"/>
+      <c r="B64" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="24"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="24"/>
-      <c r="J64" s="24"/>
-      <c r="K64" s="24"/>
-      <c r="L64" s="24"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="50"/>
+      <c r="H64" s="50"/>
+      <c r="I64" s="50"/>
+      <c r="J64" s="50"/>
+      <c r="K64" s="50"/>
+      <c r="L64" s="50"/>
+    </row>
+    <row r="65" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+    </row>
+    <row r="66" spans="1:27" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="56"/>
+      <c r="B66" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="56"/>
+      <c r="H66" s="56"/>
+      <c r="I66" s="56"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="56"/>
+      <c r="L66" s="56"/>
+    </row>
+    <row r="67" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="51"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+      <c r="K67" s="51"/>
+      <c r="L67" s="51"/>
+      <c r="M67" s="51"/>
+      <c r="N67" s="51"/>
+      <c r="O67" s="51"/>
+      <c r="P67" s="51"/>
+      <c r="Q67" s="51"/>
+      <c r="R67" s="51"/>
+      <c r="S67" s="51"/>
+      <c r="T67" s="51"/>
+      <c r="U67" s="51"/>
+      <c r="V67" s="51"/>
+      <c r="W67" s="51"/>
+      <c r="X67" s="51"/>
+      <c r="Y67" s="51"/>
+      <c r="Z67" s="51"/>
+      <c r="AA67" s="51"/>
+    </row>
+    <row r="68" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="51"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="51"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="51"/>
+      <c r="L68" s="51"/>
+      <c r="M68" s="51"/>
+      <c r="N68" s="51"/>
+      <c r="O68" s="51"/>
+      <c r="P68" s="51"/>
+      <c r="Q68" s="51"/>
+      <c r="R68" s="51"/>
+      <c r="S68" s="51"/>
+      <c r="T68" s="51"/>
+      <c r="U68" s="51"/>
+      <c r="V68" s="51"/>
+      <c r="W68" s="51"/>
+      <c r="X68" s="51"/>
+      <c r="Y68" s="51"/>
+      <c r="Z68" s="51"/>
+      <c r="AA68" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C1000 E2:E1000 G2:G1000 K2:K64 I48:I64">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1000 E2:E1000 G2:G1000 K2:K64 I48:I64">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1000">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1000">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1000">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1000">
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1000 K2:K64 I48:J64">
-    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1000 K2:K64 I48:J64">
-    <cfRule type="expression" dxfId="3" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I48:I64 K2:K64 C2:C592 E2:E592 G2:G592">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified acceptance test plan
</commit_message>
<xml_diff>
--- a/etc/WebCheckers Acceptance Test Plan - Grade A Slackers.xlsx
+++ b/etc/WebCheckers Acceptance Test Plan - Grade A Slackers.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2171-swen-261-04-b-Grade-A-Slackers\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\SWEN261\2171-swen-261-04-b-Grade-A-Slackers\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="103">
   <si>
     <t>Instructions</t>
   </si>
@@ -309,13 +309,7 @@
     <t>Given I have selected a game when I click the replay button then I expect to be taken to the game screen.</t>
   </si>
   <si>
-    <t>Given I am on the replaying board when I do nothing then I expect the game to replay automatically.</t>
-  </si>
-  <si>
     <t>Given I am on the replaying board when I try to move a piece then I expect nothing to happen.</t>
-  </si>
-  <si>
-    <t>Given I am on the replaying board when the game is some replaying then I expect to be taken back to the home.</t>
   </si>
   <si>
     <t>As a player I want to have a spectator mode available so that I may view other players' games.</t>
@@ -345,7 +339,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -645,39 +639,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -996,14 +958,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="106.875" customWidth="1"/>
+    <col min="2" max="2" width="106.83203125" customWidth="1"/>
     <col min="3" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,10 +973,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1022,7 +984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1030,55 +992,55 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
     </row>
   </sheetData>
@@ -1088,14 +1050,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA68"/>
+  <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B66" sqref="B66"/>
+      <selection pane="topRight" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="60" customWidth="1"/>
@@ -1105,14 +1067,14 @@
     <col min="6" max="6" width="60" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="60" customWidth="1"/>
-    <col min="9" max="9" width="10.875" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
     <col min="10" max="10" width="46.5" customWidth="1"/>
-    <col min="11" max="11" width="10.875" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
     <col min="12" max="12" width="36.75" customWidth="1"/>
-    <col min="13" max="18" width="10.875" customWidth="1"/>
+    <col min="13" max="18" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +1118,7 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
@@ -1191,7 +1153,7 @@
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>20</v>
@@ -1224,7 +1186,7 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -1257,7 +1219,7 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -1290,7 +1252,7 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>24</v>
@@ -1323,7 +1285,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>25</v>
@@ -1356,7 +1318,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>27</v>
@@ -1389,7 +1351,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>28</v>
@@ -1422,7 +1384,7 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>29</v>
@@ -1456,7 +1418,7 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>31</v>
       </c>
@@ -1491,7 +1453,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -1524,7 +1486,7 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>36</v>
@@ -1557,7 +1519,7 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>37</v>
@@ -1590,7 +1552,7 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>38</v>
@@ -1623,7 +1585,7 @@
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>39</v>
@@ -1656,7 +1618,7 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>40</v>
@@ -1689,7 +1651,7 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>42</v>
@@ -1723,7 +1685,7 @@
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
         <v>43</v>
       </c>
@@ -1754,7 +1716,7 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
     </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>45</v>
@@ -1783,7 +1745,7 @@
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>46</v>
@@ -1812,7 +1774,7 @@
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>47</v>
@@ -1841,7 +1803,7 @@
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="30"/>
       <c r="B23" s="30" t="s">
         <v>48</v>
@@ -1871,7 +1833,7 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
@@ -1902,7 +1864,7 @@
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
     </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>51</v>
@@ -1931,7 +1893,7 @@
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
     </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
@@ -1960,7 +1922,7 @@
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>54</v>
@@ -1989,7 +1951,7 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
     </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="30"/>
       <c r="B28" s="30" t="s">
         <v>55</v>
@@ -2019,7 +1981,7 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
     </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -2046,7 +2008,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>58</v>
@@ -2075,7 +2037,7 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
     </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>59</v>
@@ -2104,7 +2066,7 @@
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
     </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>61</v>
@@ -2133,7 +2095,7 @@
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
     </row>
-    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="30"/>
       <c r="B33" s="30" t="s">
         <v>62</v>
@@ -2163,7 +2125,7 @@
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
     </row>
-    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -2194,7 +2156,7 @@
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="39"/>
       <c r="B35" s="39" t="s">
         <v>66</v>
@@ -2219,7 +2181,7 @@
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="42"/>
       <c r="B36" s="43" t="s">
         <v>68</v>
@@ -2249,7 +2211,7 @@
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="39" t="s">
         <v>69</v>
       </c>
@@ -2276,7 +2238,7 @@
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
     </row>
-    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="46" t="s">
         <v>71</v>
       </c>
@@ -2300,7 +2262,7 @@
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
     </row>
-    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="24"/>
       <c r="B39" s="47" t="s">
         <v>72</v>
@@ -2330,7 +2292,7 @@
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
     </row>
-    <row r="40" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A40" s="46" t="s">
         <v>73</v>
       </c>
@@ -2350,7 +2312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="46" t="s">
         <v>75</v>
       </c>
@@ -2367,7 +2329,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B42" s="46" t="s">
         <v>76</v>
       </c>
@@ -2384,7 +2346,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B43" s="46" t="s">
         <v>77</v>
       </c>
@@ -2401,7 +2363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="31" x14ac:dyDescent="0.35">
       <c r="A44" s="24"/>
       <c r="B44" s="47" t="s">
         <v>78</v>
@@ -2425,7 +2387,7 @@
       <c r="K44" s="24"/>
       <c r="L44" s="24"/>
     </row>
-    <row r="45" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="62" x14ac:dyDescent="0.35">
       <c r="A45" s="46" t="s">
         <v>79</v>
       </c>
@@ -2445,7 +2407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B46" s="46" t="s">
         <v>81</v>
       </c>
@@ -2462,7 +2424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A47" s="24"/>
       <c r="B47" s="47" t="s">
         <v>82</v>
@@ -2486,7 +2448,7 @@
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
     </row>
-    <row r="48" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="62" x14ac:dyDescent="0.35">
       <c r="A48" s="48" t="s">
         <v>83</v>
       </c>
@@ -2494,22 +2456,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="B49" s="48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B50" s="48" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B51" s="48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A52" s="24"/>
       <c r="B52" s="49" t="s">
         <v>88</v>
@@ -2525,7 +2487,7 @@
       <c r="K52" s="24"/>
       <c r="L52" s="24"/>
     </row>
-    <row r="53" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A53" s="48" t="s">
         <v>89</v>
       </c>
@@ -2533,110 +2495,132 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="B54" s="48" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="B55" s="48" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="B56" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="B57" s="48" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B58" s="48" t="s">
+    <row r="58" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="54"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+    </row>
+    <row r="59" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="48" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="54"/>
-      <c r="B59" s="55" t="s">
+      <c r="B59" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C59" s="54"/>
-      <c r="D59" s="54"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="54"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
-      <c r="J59" s="24"/>
-      <c r="K59" s="24"/>
-      <c r="L59" s="24"/>
-    </row>
-    <row r="60" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="48" t="s">
+    </row>
+    <row r="60" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B60" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="48" t="s">
+    </row>
+    <row r="61" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B61" s="48" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B61" s="48" t="s">
+    <row r="62" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="B62" s="48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B62" s="48" t="s">
+    <row r="63" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="50"/>
+      <c r="B63" s="52" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B63" s="48" t="s">
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="50"/>
+      <c r="H63" s="50"/>
+      <c r="I63" s="50"/>
+      <c r="J63" s="50"/>
+      <c r="K63" s="50"/>
+      <c r="L63" s="50"/>
+    </row>
+    <row r="64" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="53" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="50"/>
-      <c r="B64" s="52" t="s">
+      <c r="G64" s="51"/>
+      <c r="H64" s="51"/>
+    </row>
+    <row r="65" spans="1:27" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="56"/>
+      <c r="B65" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="C64" s="50"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="50"/>
-      <c r="G64" s="50"/>
-      <c r="H64" s="50"/>
-      <c r="I64" s="50"/>
-      <c r="J64" s="50"/>
-      <c r="K64" s="50"/>
-      <c r="L64" s="50"/>
-    </row>
-    <row r="65" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="G65" s="51"/>
-      <c r="H65" s="51"/>
-    </row>
-    <row r="66" spans="1:27" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="56"/>
-      <c r="B66" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="56"/>
-      <c r="I66" s="56"/>
-      <c r="J66" s="56"/>
-      <c r="K66" s="56"/>
-      <c r="L66" s="56"/>
-    </row>
-    <row r="67" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
+      <c r="H65" s="56"/>
+      <c r="I65" s="56"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="56"/>
+      <c r="L65" s="56"/>
+    </row>
+    <row r="66" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="51"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="51"/>
+      <c r="L66" s="51"/>
+      <c r="M66" s="51"/>
+      <c r="N66" s="51"/>
+      <c r="O66" s="51"/>
+      <c r="P66" s="51"/>
+      <c r="Q66" s="51"/>
+      <c r="R66" s="51"/>
+      <c r="S66" s="51"/>
+      <c r="T66" s="51"/>
+      <c r="U66" s="51"/>
+      <c r="V66" s="51"/>
+      <c r="W66" s="51"/>
+      <c r="X66" s="51"/>
+      <c r="Y66" s="51"/>
+      <c r="Z66" s="51"/>
+      <c r="AA66" s="51"/>
+    </row>
+    <row r="67" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="51"/>
       <c r="B67" s="51"/>
       <c r="C67" s="51"/>
@@ -2665,78 +2649,29 @@
       <c r="Z67" s="51"/>
       <c r="AA67" s="51"/>
     </row>
-    <row r="68" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="51"/>
-      <c r="B68" s="51"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="51"/>
-      <c r="E68" s="51"/>
-      <c r="F68" s="51"/>
-      <c r="G68" s="51"/>
-      <c r="H68" s="51"/>
-      <c r="I68" s="51"/>
-      <c r="J68" s="51"/>
-      <c r="K68" s="51"/>
-      <c r="L68" s="51"/>
-      <c r="M68" s="51"/>
-      <c r="N68" s="51"/>
-      <c r="O68" s="51"/>
-      <c r="P68" s="51"/>
-      <c r="Q68" s="51"/>
-      <c r="R68" s="51"/>
-      <c r="S68" s="51"/>
-      <c r="T68" s="51"/>
-      <c r="U68" s="51"/>
-      <c r="V68" s="51"/>
-      <c r="W68" s="51"/>
-      <c r="X68" s="51"/>
-      <c r="Y68" s="51"/>
-      <c r="Z68" s="51"/>
-      <c r="AA68" s="51"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1000 E2:E1000 G2:G1000 K2:K64 I48:I64">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+  <conditionalFormatting sqref="C2:C999 E2:E999 G2:G999 K2:K63 I48:I63">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1000 E2:E1000 G2:G1000 K2:K64 I48:I64">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C999 E2:E999 G2:G999 K2:K63 I48:I63">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1000">
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D999 F2:F999 H2:H999 K2:K63 I48:J63">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D1000">
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D999 F2:F999 H2:H999 K2:K63 I48:J63">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1000">
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
-      <formula>AND(ISBLANK(F2),E2="Pass")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F1000">
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
-      <formula>AND(ISBLANK(F2),E2="Fail")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1000 K2:K64 I48:J64">
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
-      <formula>AND(ISBLANK(H2),G2="Pass")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1000 K2:K64 I48:J64">
-    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
-      <formula>AND(ISBLANK(H2),G2="Fail")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I48:I64 K2:K64 C2:C592 E2:E592 G2:G592">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G591 E2:E591 C2:C591 K2:K63 I48:I63">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>